<commit_message>
Implementación de subsedes regionales y actualización de consultas para reportes.
</commit_message>
<xml_diff>
--- a/public/templates/PIRConsolidado.xlsx
+++ b/public/templates/PIRConsolidado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="495" windowWidth="23415" windowHeight="9405" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="23415" windowHeight="9405" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PERSONAL 0" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Personal!$1:$14</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -233,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -243,79 +242,99 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="7"/>
       <color rgb="FF10253F"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF10253F"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -734,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -917,9 +936,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1045,9 +1061,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1223,6 +1236,31 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1238,32 +1276,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1278,46 +1298,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,15 +1356,6 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1361,14 +1383,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1396,7 +1424,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1439,7 +1467,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1482,7 +1510,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="3 Imagen"/>
+        <xdr:cNvPr id="2" name="3 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1524,7 +1552,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="3 Imagen"/>
+        <xdr:cNvPr id="2" name="3 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1916,28 +1944,28 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="207" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="207"/>
-      <c r="C10" s="207"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207"/>
-      <c r="G10" s="207"/>
+      <c r="A10" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="201"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="201"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A11" s="207" t="s">
+      <c r="A11" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="207"/>
-      <c r="C11" s="207"/>
-      <c r="D11" s="207"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="207"/>
-      <c r="G11" s="207"/>
+      <c r="B11" s="201"/>
+      <c r="C11" s="201"/>
+      <c r="D11" s="201"/>
+      <c r="E11" s="201"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="201"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
@@ -1953,28 +1981,28 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="199" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="205"/>
-      <c r="C13" s="205"/>
-      <c r="D13" s="205"/>
-      <c r="E13" s="205"/>
-      <c r="F13" s="205"/>
-      <c r="G13" s="205"/>
+      <c r="B13" s="199"/>
+      <c r="C13" s="199"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="199"/>
+      <c r="G13" s="199"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A14" s="206" t="s">
+      <c r="A14" s="200" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="206"/>
-      <c r="C14" s="206"/>
-      <c r="D14" s="206"/>
-      <c r="E14" s="206"/>
-      <c r="F14" s="206"/>
-      <c r="G14" s="206"/>
+      <c r="B14" s="200"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="200"/>
+      <c r="E14" s="200"/>
+      <c r="F14" s="200"/>
+      <c r="G14" s="200"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
     </row>
@@ -1994,61 +2022,61 @@
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="212"/>
-      <c r="E16" s="212"/>
-      <c r="F16" s="212"/>
-      <c r="G16" s="212"/>
+      <c r="D16" s="197"/>
+      <c r="E16" s="197"/>
+      <c r="F16" s="197"/>
+      <c r="G16" s="197"/>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="209"/>
-      <c r="B17" s="210" t="s">
+      <c r="A17" s="196"/>
+      <c r="B17" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="208" t="s">
+      <c r="C17" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="208" t="s">
+      <c r="D17" s="202" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="208" t="s">
+      <c r="E17" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="208" t="s">
+      <c r="F17" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="208" t="s">
+      <c r="G17" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="209"/>
-      <c r="I17" s="209"/>
+      <c r="H17" s="196"/>
+      <c r="I17" s="196"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="209"/>
-      <c r="B18" s="210"/>
-      <c r="C18" s="208"/>
-      <c r="D18" s="208"/>
-      <c r="E18" s="208"/>
-      <c r="F18" s="208"/>
-      <c r="G18" s="208"/>
-      <c r="H18" s="209"/>
-      <c r="I18" s="209"/>
+      <c r="A18" s="196"/>
+      <c r="B18" s="203"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="202"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="196"/>
+      <c r="I18" s="196"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1">
-      <c r="A19" s="209"/>
-      <c r="B19" s="211"/>
-      <c r="C19" s="208"/>
-      <c r="D19" s="208"/>
-      <c r="E19" s="208"/>
-      <c r="F19" s="208"/>
-      <c r="G19" s="208"/>
-      <c r="H19" s="209"/>
-      <c r="I19" s="209"/>
+      <c r="A19" s="196"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="196"/>
+      <c r="I19" s="196"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1">
-      <c r="A20" s="209"/>
-      <c r="B20" s="204">
+      <c r="A20" s="196"/>
+      <c r="B20" s="210">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
@@ -2068,15 +2096,15 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="9.75" customHeight="1">
-      <c r="A21" s="209"/>
-      <c r="B21" s="204"/>
-      <c r="C21" s="201" t="s">
+      <c r="A21" s="196"/>
+      <c r="B21" s="210"/>
+      <c r="C21" s="208" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="202"/>
-      <c r="E21" s="203"/>
-      <c r="F21" s="203"/>
-      <c r="G21" s="200"/>
+      <c r="D21" s="209"/>
+      <c r="E21" s="198"/>
+      <c r="F21" s="198"/>
+      <c r="G21" s="207"/>
       <c r="H21" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2087,13 +2115,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="7.5" customHeight="1">
-      <c r="A22" s="209"/>
-      <c r="B22" s="204"/>
-      <c r="C22" s="201"/>
-      <c r="D22" s="202"/>
-      <c r="E22" s="203"/>
-      <c r="F22" s="203"/>
-      <c r="G22" s="200"/>
+      <c r="A22" s="196"/>
+      <c r="B22" s="210"/>
+      <c r="C22" s="208"/>
+      <c r="D22" s="209"/>
+      <c r="E22" s="198"/>
+      <c r="F22" s="198"/>
+      <c r="G22" s="207"/>
       <c r="H22" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2104,8 +2132,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
-      <c r="A23" s="209"/>
-      <c r="B23" s="204"/>
+      <c r="A23" s="196"/>
+      <c r="B23" s="210"/>
       <c r="C23" s="21" t="s">
         <v>14</v>
       </c>
@@ -2123,8 +2151,8 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
-      <c r="A24" s="209"/>
-      <c r="B24" s="204"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="210"/>
       <c r="C24" s="21" t="s">
         <v>15</v>
       </c>
@@ -2142,8 +2170,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1">
-      <c r="A25" s="209"/>
-      <c r="B25" s="204"/>
+      <c r="A25" s="196"/>
+      <c r="B25" s="210"/>
       <c r="C25" s="21" t="s">
         <v>16</v>
       </c>
@@ -2161,8 +2189,8 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1">
-      <c r="A26" s="209"/>
-      <c r="B26" s="204"/>
+      <c r="A26" s="196"/>
+      <c r="B26" s="210"/>
       <c r="C26" s="21" t="s">
         <v>17</v>
       </c>
@@ -2180,8 +2208,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1">
-      <c r="A27" s="209"/>
-      <c r="B27" s="204"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="210"/>
       <c r="C27" s="21" t="s">
         <v>18</v>
       </c>
@@ -2199,8 +2227,8 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1">
-      <c r="A28" s="209"/>
-      <c r="B28" s="204"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="210"/>
       <c r="C28" s="21" t="s">
         <v>19</v>
       </c>
@@ -2218,8 +2246,8 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1">
-      <c r="A29" s="209"/>
-      <c r="B29" s="204"/>
+      <c r="A29" s="196"/>
+      <c r="B29" s="210"/>
       <c r="C29" s="21" t="s">
         <v>20</v>
       </c>
@@ -2348,10 +2376,10 @@
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1">
       <c r="A35" s="7"/>
-      <c r="B35" s="198" t="s">
+      <c r="B35" s="205" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="199"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="31">
         <f>SUM(D20:D34)</f>
         <v>0</v>
@@ -2476,11 +2504,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="22">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B20:B29"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A10:G10"/>
@@ -2492,12 +2521,11 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B20:B29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="H17:H19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.54500000000000004" bottom="0" header="0.51180555555555995" footer="0.51180555555555995"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
@@ -2599,29 +2627,29 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A9" s="207" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="207"/>
-      <c r="C9" s="207"/>
-      <c r="D9" s="207"/>
-      <c r="E9" s="207"/>
-      <c r="F9" s="207"/>
-      <c r="G9" s="207"/>
+      <c r="A9" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="201"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="201"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A10" s="207" t="s">
+      <c r="A10" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="207"/>
-      <c r="C10" s="207"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="201"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="201"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2639,31 +2667,31 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A12" s="207" t="s">
+      <c r="A12" s="201" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="207"/>
-      <c r="C12" s="207"/>
-      <c r="D12" s="207"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="207"/>
-      <c r="G12" s="207"/>
-      <c r="H12" s="207"/>
-      <c r="I12" s="207"/>
+      <c r="B12" s="201"/>
+      <c r="C12" s="201"/>
+      <c r="D12" s="201"/>
+      <c r="E12" s="201"/>
+      <c r="F12" s="201"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="201"/>
+      <c r="I12" s="201"/>
       <c r="J12" s="36"/>
     </row>
     <row r="13" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A13" s="213" t="s">
+      <c r="A13" s="214" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="213"/>
-      <c r="C13" s="213"/>
-      <c r="D13" s="213"/>
-      <c r="E13" s="213"/>
-      <c r="F13" s="213"/>
-      <c r="G13" s="213"/>
-      <c r="H13" s="213"/>
-      <c r="I13" s="213"/>
+      <c r="B13" s="214"/>
+      <c r="C13" s="214"/>
+      <c r="D13" s="214"/>
+      <c r="E13" s="214"/>
+      <c r="F13" s="214"/>
+      <c r="G13" s="214"/>
+      <c r="H13" s="214"/>
+      <c r="I13" s="214"/>
       <c r="J13" s="36"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" customHeight="1">
@@ -2685,65 +2713,65 @@
       <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="212"/>
-      <c r="E15" s="212"/>
-      <c r="F15" s="212"/>
-      <c r="G15" s="212"/>
+      <c r="D15" s="197"/>
+      <c r="E15" s="197"/>
+      <c r="F15" s="197"/>
+      <c r="G15" s="197"/>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A16" s="209"/>
-      <c r="B16" s="210" t="s">
+      <c r="A16" s="196"/>
+      <c r="B16" s="203" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="208" t="s">
+      <c r="C16" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="208" t="s">
+      <c r="D16" s="202" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="208" t="s">
+      <c r="E16" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="208" t="s">
+      <c r="F16" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="208" t="s">
+      <c r="G16" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="209"/>
-      <c r="I16" s="209"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="196"/>
       <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A17" s="209"/>
-      <c r="B17" s="210"/>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
-      <c r="E17" s="208"/>
-      <c r="F17" s="208"/>
-      <c r="G17" s="208"/>
-      <c r="H17" s="209"/>
-      <c r="I17" s="209"/>
+      <c r="A17" s="196"/>
+      <c r="B17" s="203"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="202"/>
+      <c r="E17" s="202"/>
+      <c r="F17" s="202"/>
+      <c r="G17" s="202"/>
+      <c r="H17" s="196"/>
+      <c r="I17" s="196"/>
       <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1">
-      <c r="A18" s="209"/>
-      <c r="B18" s="210"/>
-      <c r="C18" s="208"/>
-      <c r="D18" s="208"/>
-      <c r="E18" s="208"/>
-      <c r="F18" s="208"/>
-      <c r="G18" s="208"/>
-      <c r="H18" s="209"/>
-      <c r="I18" s="209"/>
+      <c r="A18" s="196"/>
+      <c r="B18" s="203"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="202"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="202"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="196"/>
+      <c r="I18" s="196"/>
       <c r="J18" s="37"/>
     </row>
     <row r="19" spans="1:12" ht="18" customHeight="1">
-      <c r="A19" s="209"/>
-      <c r="B19" s="214">
+      <c r="A19" s="196"/>
+      <c r="B19" s="215">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2772,15 +2800,15 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A20" s="209"/>
-      <c r="B20" s="215"/>
-      <c r="C20" s="219" t="s">
+      <c r="A20" s="196"/>
+      <c r="B20" s="216"/>
+      <c r="C20" s="211" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="202"/>
-      <c r="E20" s="203"/>
-      <c r="F20" s="203"/>
-      <c r="G20" s="200"/>
+      <c r="D20" s="209"/>
+      <c r="E20" s="198"/>
+      <c r="F20" s="198"/>
+      <c r="G20" s="207"/>
       <c r="H20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2800,13 +2828,13 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A21" s="209"/>
-      <c r="B21" s="215"/>
-      <c r="C21" s="219"/>
-      <c r="D21" s="202"/>
-      <c r="E21" s="203"/>
-      <c r="F21" s="203"/>
-      <c r="G21" s="200"/>
+      <c r="A21" s="196"/>
+      <c r="B21" s="216"/>
+      <c r="C21" s="211"/>
+      <c r="D21" s="209"/>
+      <c r="E21" s="198"/>
+      <c r="F21" s="198"/>
+      <c r="G21" s="207"/>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2826,8 +2854,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1">
-      <c r="A22" s="209"/>
-      <c r="B22" s="215"/>
+      <c r="A22" s="196"/>
+      <c r="B22" s="216"/>
       <c r="C22" s="18" t="s">
         <v>14</v>
       </c>
@@ -2854,8 +2882,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.5" customHeight="1">
-      <c r="A23" s="209"/>
-      <c r="B23" s="215"/>
+      <c r="A23" s="196"/>
+      <c r="B23" s="216"/>
       <c r="C23" s="18" t="s">
         <v>15</v>
       </c>
@@ -2882,8 +2910,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="18" customHeight="1">
-      <c r="A24" s="209"/>
-      <c r="B24" s="215"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="18" t="s">
         <v>16</v>
       </c>
@@ -2910,8 +2938,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="18" customHeight="1">
-      <c r="A25" s="209"/>
-      <c r="B25" s="215"/>
+      <c r="A25" s="196"/>
+      <c r="B25" s="216"/>
       <c r="C25" s="18" t="s">
         <v>17</v>
       </c>
@@ -2939,7 +2967,7 @@
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="216"/>
+      <c r="B26" s="217"/>
       <c r="C26" s="18" t="s">
         <v>20</v>
       </c>
@@ -3121,10 +3149,10 @@
     </row>
     <row r="32" spans="1:12" s="34" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="30"/>
-      <c r="B32" s="217" t="s">
+      <c r="B32" s="212" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="218"/>
+      <c r="C32" s="213"/>
       <c r="D32" s="31">
         <f>SUM(D19:D31)</f>
         <v>0</v>
@@ -3267,12 +3295,13 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="21">
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B19:B26"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="H16:H18"/>
     <mergeCell ref="E20:E21"/>
@@ -3281,13 +3310,12 @@
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3299,9 +3327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:P59"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16:G18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3326,63 +3354,63 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="220"/>
-      <c r="C7" s="220"/>
-      <c r="D7" s="220"/>
-      <c r="E7" s="220"/>
-      <c r="F7" s="220"/>
-      <c r="G7" s="220"/>
-      <c r="H7" s="220"/>
-      <c r="I7" s="220"/>
-      <c r="J7" s="220"/>
+      <c r="A7" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="227"/>
+      <c r="C7" s="227"/>
+      <c r="D7" s="227"/>
+      <c r="E7" s="227"/>
+      <c r="F7" s="227"/>
+      <c r="G7" s="227"/>
+      <c r="H7" s="227"/>
+      <c r="I7" s="227"/>
+      <c r="J7" s="227"/>
       <c r="K7" s="46"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="227" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="220"/>
-      <c r="C8" s="220"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="220"/>
-      <c r="F8" s="220"/>
-      <c r="G8" s="220"/>
-      <c r="H8" s="220"/>
-      <c r="I8" s="220"/>
-      <c r="J8" s="220"/>
+      <c r="B8" s="227"/>
+      <c r="C8" s="227"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="227"/>
+      <c r="G8" s="227"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="227"/>
       <c r="K8" s="46"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="220" t="s">
+      <c r="A9" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="220"/>
-      <c r="C9" s="220"/>
-      <c r="D9" s="220"/>
-      <c r="E9" s="220"/>
-      <c r="F9" s="220"/>
-      <c r="G9" s="220"/>
-      <c r="H9" s="220"/>
-      <c r="I9" s="220"/>
-      <c r="J9" s="220"/>
+      <c r="B9" s="227"/>
+      <c r="C9" s="227"/>
+      <c r="D9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="227"/>
+      <c r="H9" s="227"/>
+      <c r="I9" s="227"/>
+      <c r="J9" s="227"/>
       <c r="K9" s="46"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="220" t="s">
+      <c r="A10" s="227" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="220"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="220"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="220"/>
+      <c r="B10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="227"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="227"/>
       <c r="K10" s="46"/>
     </row>
     <row r="11" spans="1:12">
@@ -3390,13 +3418,13 @@
       <c r="B11" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="105"/>
+      <c r="C11" s="104"/>
       <c r="D11" s="77"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
       <c r="H11" s="47"/>
-      <c r="I11" s="121" t="s">
+      <c r="I11" s="120" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="43"/>
@@ -3404,219 +3432,219 @@
       <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="222" t="s">
+      <c r="A12" s="228" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="224" t="s">
+      <c r="B12" s="222" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="224" t="s">
+      <c r="C12" s="222" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="224" t="s">
+      <c r="D12" s="222" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="224" t="s">
+      <c r="E12" s="222" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="225" t="s">
+      <c r="F12" s="220" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="225" t="s">
+      <c r="G12" s="220" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="225" t="s">
+      <c r="H12" s="220" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="225" t="s">
+      <c r="I12" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="224" t="s">
+      <c r="J12" s="222" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="221"/>
-      <c r="L12" s="221"/>
+      <c r="K12" s="223"/>
+      <c r="L12" s="223"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="222"/>
-      <c r="B13" s="224"/>
-      <c r="C13" s="224"/>
-      <c r="D13" s="224"/>
-      <c r="E13" s="224"/>
-      <c r="F13" s="226"/>
-      <c r="G13" s="226"/>
-      <c r="H13" s="226"/>
-      <c r="I13" s="226"/>
-      <c r="J13" s="224"/>
-      <c r="K13" s="221"/>
-      <c r="L13" s="221"/>
+      <c r="A13" s="228"/>
+      <c r="B13" s="222"/>
+      <c r="C13" s="222"/>
+      <c r="D13" s="222"/>
+      <c r="E13" s="222"/>
+      <c r="F13" s="221"/>
+      <c r="G13" s="221"/>
+      <c r="H13" s="221"/>
+      <c r="I13" s="221"/>
+      <c r="J13" s="222"/>
+      <c r="K13" s="223"/>
+      <c r="L13" s="223"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A14" s="223"/>
-      <c r="B14" s="225"/>
-      <c r="C14" s="225"/>
-      <c r="D14" s="225"/>
-      <c r="E14" s="225"/>
-      <c r="F14" s="226"/>
-      <c r="G14" s="226"/>
-      <c r="H14" s="226"/>
-      <c r="I14" s="226"/>
-      <c r="J14" s="225"/>
-      <c r="K14" s="221"/>
-      <c r="L14" s="221"/>
+      <c r="A14" s="229"/>
+      <c r="B14" s="220"/>
+      <c r="C14" s="220"/>
+      <c r="D14" s="220"/>
+      <c r="E14" s="220"/>
+      <c r="F14" s="221"/>
+      <c r="G14" s="221"/>
+      <c r="H14" s="221"/>
+      <c r="I14" s="221"/>
+      <c r="J14" s="220"/>
+      <c r="K14" s="223"/>
+      <c r="L14" s="223"/>
     </row>
     <row r="15" spans="1:12" s="72" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="229">
+      <c r="A15" s="224">
         <v>1</v>
       </c>
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="129">
+      <c r="C15" s="127">
         <f>SUM(D15:G15)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="129">
+      <c r="D15" s="127">
         <f>SUM(D16:D18)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="129">
+      <c r="E15" s="127">
         <f>SUM(E16:E18)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="129">
+      <c r="F15" s="127">
         <f>SUM(F16:F18)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="129">
+      <c r="G15" s="127">
         <f>SUM(G16:G18)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
-      <c r="J15" s="131"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="129"/>
       <c r="K15" s="73"/>
     </row>
     <row r="16" spans="1:12" s="72" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="229"/>
-      <c r="B16" s="139" t="s">
+      <c r="A16" s="224"/>
+      <c r="B16" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="129">
+      <c r="C16" s="127">
         <f>SUM(D16:G16)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="127"/>
-      <c r="E16" s="128"/>
-      <c r="F16" s="128"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
+      <c r="D16" s="248"/>
+      <c r="E16" s="248"/>
+      <c r="F16" s="248"/>
+      <c r="G16" s="248"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="126"/>
+      <c r="J16" s="126"/>
       <c r="K16" s="73"/>
     </row>
     <row r="17" spans="1:16" s="72" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="229"/>
-      <c r="B17" s="140" t="s">
+      <c r="A17" s="224"/>
+      <c r="B17" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="129">
+      <c r="C17" s="127">
         <f>SUM(D17:G17)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
+      <c r="D17" s="249"/>
+      <c r="E17" s="249"/>
+      <c r="F17" s="249"/>
+      <c r="G17" s="249"/>
       <c r="H17" s="58"/>
-      <c r="I17" s="83"/>
+      <c r="I17" s="82"/>
       <c r="J17" s="48"/>
       <c r="K17" s="73"/>
     </row>
     <row r="18" spans="1:16" s="72" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="229"/>
-      <c r="B18" s="140" t="s">
+      <c r="A18" s="224"/>
+      <c r="B18" s="138" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="129">
+      <c r="C18" s="127">
         <f>SUM(D18:G18)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
+      <c r="D18" s="249"/>
+      <c r="E18" s="249"/>
+      <c r="F18" s="249"/>
+      <c r="G18" s="249"/>
       <c r="H18" s="57"/>
       <c r="I18" s="76"/>
       <c r="J18" s="48"/>
       <c r="K18" s="73"/>
     </row>
     <row r="19" spans="1:16" s="72" customFormat="1">
-      <c r="A19" s="229"/>
-      <c r="B19" s="141" t="s">
+      <c r="A19" s="224"/>
+      <c r="B19" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="84">
+      <c r="C19" s="83">
         <f>SUM(C21,C23,C24,C26,C27,C29,C31)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="84">
+      <c r="D19" s="83">
         <f>SUM(D21,D23,D24,D26,D27,D29,D31)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="84">
+      <c r="E19" s="83">
         <f>SUM(E21,E23,E24,E26,E27,E29,E31)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="84">
+      <c r="F19" s="83">
         <f>SUM(F21,F23,F24,F26,F27,F29,F31)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="84">
+      <c r="G19" s="83">
         <f>SUM(G21,G23,G24,G26,G27,G29,G31)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="84"/>
+      <c r="H19" s="83"/>
       <c r="I19" s="79"/>
       <c r="J19" s="79"/>
       <c r="K19" s="73"/>
     </row>
     <row r="20" spans="1:16" s="72" customFormat="1">
-      <c r="A20" s="229"/>
-      <c r="B20" s="231" t="s">
+      <c r="A20" s="224"/>
+      <c r="B20" s="226" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="231"/>
-      <c r="H20" s="231"/>
-      <c r="I20" s="231"/>
-      <c r="J20" s="85"/>
+      <c r="C20" s="226"/>
+      <c r="D20" s="226"/>
+      <c r="E20" s="226"/>
+      <c r="F20" s="226"/>
+      <c r="G20" s="226"/>
+      <c r="H20" s="226"/>
+      <c r="I20" s="226"/>
+      <c r="J20" s="84"/>
       <c r="K20" s="73"/>
     </row>
     <row r="21" spans="1:16" s="66" customFormat="1">
-      <c r="A21" s="229"/>
-      <c r="B21" s="98" t="s">
+      <c r="A21" s="224"/>
+      <c r="B21" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="110">
+      <c r="C21" s="109">
         <f>SUM(D21:G21)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="137"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="247"/>
+      <c r="F21" s="247"/>
+      <c r="G21" s="247"/>
+      <c r="H21" s="132"/>
+      <c r="I21" s="135"/>
       <c r="J21" s="64"/>
       <c r="K21" s="69"/>
     </row>
     <row r="22" spans="1:16" s="66" customFormat="1">
-      <c r="A22" s="229"/>
-      <c r="B22" s="142" t="s">
+      <c r="A22" s="224"/>
+      <c r="B22" s="140" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="69"/>
@@ -3626,99 +3654,99 @@
       <c r="G22" s="69"/>
       <c r="H22" s="69"/>
       <c r="I22" s="69"/>
-      <c r="J22" s="125"/>
+      <c r="J22" s="124"/>
       <c r="K22" s="69"/>
     </row>
     <row r="23" spans="1:16" s="66" customFormat="1">
-      <c r="A23" s="229"/>
-      <c r="B23" s="98" t="s">
+      <c r="A23" s="224"/>
+      <c r="B23" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="110">
+      <c r="C23" s="109">
         <f>SUM(D23:G23)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="137"/>
+      <c r="D23" s="247"/>
+      <c r="E23" s="247"/>
+      <c r="F23" s="247"/>
+      <c r="G23" s="247"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="135"/>
       <c r="J23" s="64"/>
       <c r="K23" s="69"/>
     </row>
     <row r="24" spans="1:16" s="66" customFormat="1">
-      <c r="A24" s="229"/>
-      <c r="B24" s="143" t="s">
+      <c r="A24" s="224"/>
+      <c r="B24" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="123">
+      <c r="C24" s="122">
         <f>SUM(D24:G24)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="134"/>
-      <c r="I24" s="137"/>
-      <c r="J24" s="124"/>
+      <c r="D24" s="250"/>
+      <c r="E24" s="250"/>
+      <c r="F24" s="250"/>
+      <c r="G24" s="250"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="123"/>
       <c r="K24" s="69"/>
     </row>
     <row r="25" spans="1:16" s="66" customFormat="1">
-      <c r="A25" s="229"/>
-      <c r="B25" s="144" t="s">
+      <c r="A25" s="224"/>
+      <c r="B25" s="142" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
-      <c r="H25" s="132"/>
-      <c r="I25" s="132"/>
-      <c r="J25" s="126"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="125"/>
       <c r="K25" s="69"/>
     </row>
     <row r="26" spans="1:16" s="66" customFormat="1">
-      <c r="A26" s="229"/>
-      <c r="B26" s="114" t="s">
+      <c r="A26" s="224"/>
+      <c r="B26" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="133">
+      <c r="C26" s="131">
         <f>SUM(D26:G26)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="134"/>
-      <c r="I26" s="137"/>
+      <c r="D26" s="251"/>
+      <c r="E26" s="251"/>
+      <c r="F26" s="251"/>
+      <c r="G26" s="251"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="135"/>
       <c r="J26" s="67"/>
       <c r="K26" s="69"/>
     </row>
     <row r="27" spans="1:16" s="66" customFormat="1">
-      <c r="A27" s="229"/>
-      <c r="B27" s="98" t="s">
+      <c r="A27" s="224"/>
+      <c r="B27" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="110">
+      <c r="C27" s="109">
         <f>SUM(D27:G27)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="134"/>
-      <c r="I27" s="137"/>
+      <c r="D27" s="247"/>
+      <c r="E27" s="247"/>
+      <c r="F27" s="247"/>
+      <c r="G27" s="247"/>
+      <c r="H27" s="132"/>
+      <c r="I27" s="135"/>
       <c r="J27" s="64"/>
       <c r="K27" s="69"/>
     </row>
     <row r="28" spans="1:16" s="66" customFormat="1">
-      <c r="A28" s="229"/>
-      <c r="B28" s="142" t="s">
+      <c r="A28" s="224"/>
+      <c r="B28" s="140" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="73"/>
@@ -3728,30 +3756,30 @@
       <c r="G28" s="73"/>
       <c r="H28" s="73"/>
       <c r="I28" s="73"/>
-      <c r="J28" s="101"/>
+      <c r="J28" s="100"/>
       <c r="K28" s="69"/>
     </row>
     <row r="29" spans="1:16" s="66" customFormat="1">
-      <c r="A29" s="229"/>
-      <c r="B29" s="98" t="s">
+      <c r="A29" s="224"/>
+      <c r="B29" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="110">
+      <c r="C29" s="109">
         <f>SUM(D29:G29)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="134"/>
-      <c r="I29" s="137"/>
+      <c r="D29" s="247"/>
+      <c r="E29" s="247"/>
+      <c r="F29" s="247"/>
+      <c r="G29" s="247"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="135"/>
       <c r="J29" s="64"/>
       <c r="K29" s="69"/>
     </row>
     <row r="30" spans="1:16" s="66" customFormat="1">
-      <c r="A30" s="229"/>
-      <c r="B30" s="145" t="s">
+      <c r="A30" s="224"/>
+      <c r="B30" s="143" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="73"/>
@@ -3761,404 +3789,404 @@
       <c r="G30" s="73"/>
       <c r="H30" s="73"/>
       <c r="I30" s="73"/>
-      <c r="J30" s="101"/>
+      <c r="J30" s="100"/>
       <c r="K30" s="69"/>
     </row>
     <row r="31" spans="1:16" s="72" customFormat="1">
-      <c r="A31" s="230"/>
-      <c r="B31" s="140" t="s">
+      <c r="A31" s="225"/>
+      <c r="B31" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="110">
+      <c r="C31" s="109">
         <f>SUM(D31:G31)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="134"/>
-      <c r="I31" s="137"/>
+      <c r="D31" s="247"/>
+      <c r="E31" s="247"/>
+      <c r="F31" s="247"/>
+      <c r="G31" s="247"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="135"/>
       <c r="J31" s="71"/>
       <c r="K31" s="73"/>
-      <c r="O31" s="101"/>
+      <c r="O31" s="100"/>
       <c r="P31" s="73"/>
     </row>
     <row r="32" spans="1:16" s="72" customFormat="1">
-      <c r="A32" s="86">
+      <c r="A32" s="85">
         <f>+A15+1</f>
         <v>2</v>
       </c>
-      <c r="B32" s="146" t="s">
+      <c r="B32" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="84">
+      <c r="C32" s="83">
         <f>SUM(D32:G32)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="84">
+      <c r="D32" s="83">
         <f>SUM(D33)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="84">
+      <c r="E32" s="83">
         <f>SUM(E33)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="84">
+      <c r="F32" s="83">
         <f>SUM(F33)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="84">
+      <c r="G32" s="83">
         <f>SUM(G33)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="84"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="87"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
       <c r="K32" s="73"/>
     </row>
     <row r="33" spans="1:12" s="66" customFormat="1" ht="30" customHeight="1">
-      <c r="A33" s="97"/>
-      <c r="B33" s="98" t="s">
+      <c r="A33" s="96"/>
+      <c r="B33" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="110">
+      <c r="C33" s="109">
         <f>SUM(D33:G33)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="134"/>
-      <c r="I33" s="137"/>
-      <c r="J33" s="99"/>
+      <c r="D33" s="247"/>
+      <c r="E33" s="247"/>
+      <c r="F33" s="247"/>
+      <c r="G33" s="247"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="135"/>
+      <c r="J33" s="98"/>
       <c r="K33" s="68"/>
     </row>
     <row r="34" spans="1:12" s="72" customFormat="1">
-      <c r="A34" s="88">
+      <c r="A34" s="87">
         <f>+A32+1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="146" t="s">
+      <c r="B34" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="84">
+      <c r="C34" s="83">
         <f>SUM(C35)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="84">
+      <c r="D34" s="83">
         <f>SUM(D35)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="84">
+      <c r="E34" s="83">
         <f>SUM(E35)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="84">
+      <c r="F34" s="83">
         <f>SUM(F35)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="84">
+      <c r="G34" s="83">
         <f>SUM(G35)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="89"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="87"/>
+      <c r="H34" s="88"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="86"/>
       <c r="K34" s="73"/>
     </row>
     <row r="35" spans="1:12" s="66" customFormat="1">
-      <c r="A35" s="100"/>
-      <c r="B35" s="102" t="s">
+      <c r="A35" s="99"/>
+      <c r="B35" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="110">
+      <c r="C35" s="109">
         <f>SUM(D35:G35)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="134"/>
-      <c r="I35" s="137"/>
-      <c r="J35" s="99"/>
+      <c r="D35" s="247"/>
+      <c r="E35" s="247"/>
+      <c r="F35" s="247"/>
+      <c r="G35" s="247"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="135"/>
+      <c r="J35" s="98"/>
       <c r="K35" s="69"/>
     </row>
     <row r="36" spans="1:12" s="72" customFormat="1">
-      <c r="A36" s="88">
+      <c r="A36" s="87">
         <f>+A34+1</f>
         <v>4</v>
       </c>
-      <c r="B36" s="146" t="s">
+      <c r="B36" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="84">
+      <c r="C36" s="83">
         <f>+C37</f>
         <v>0</v>
       </c>
-      <c r="D36" s="84">
+      <c r="D36" s="83">
         <f>SUM(D37)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="84">
+      <c r="E36" s="83">
         <f>SUM(E37)</f>
         <v>0</v>
       </c>
-      <c r="F36" s="84">
+      <c r="F36" s="83">
         <f>SUM(F37)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="84">
+      <c r="G36" s="83">
         <f>SUM(G37)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="89"/>
-      <c r="I36" s="90"/>
-      <c r="J36" s="87"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="86"/>
       <c r="K36" s="73"/>
     </row>
     <row r="37" spans="1:12" s="66" customFormat="1">
-      <c r="A37" s="100"/>
-      <c r="B37" s="98" t="s">
+      <c r="A37" s="99"/>
+      <c r="B37" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="110">
+      <c r="C37" s="109">
         <f>SUM(D37:G37)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="134"/>
-      <c r="I37" s="137"/>
-      <c r="J37" s="99"/>
+      <c r="D37" s="247"/>
+      <c r="E37" s="247"/>
+      <c r="F37" s="247"/>
+      <c r="G37" s="247"/>
+      <c r="H37" s="132"/>
+      <c r="I37" s="135"/>
+      <c r="J37" s="98"/>
       <c r="K37" s="69"/>
     </row>
     <row r="38" spans="1:12" s="72" customFormat="1">
-      <c r="A38" s="88">
+      <c r="A38" s="87">
         <f>+A36+1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="146" t="s">
+      <c r="B38" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="84">
+      <c r="C38" s="83">
         <f>SUM(C39:C42)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="84">
+      <c r="D38" s="83">
         <f>SUM(D39:D42)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="84">
+      <c r="E38" s="83">
         <f>SUM(E39:E42)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="84">
+      <c r="F38" s="83">
         <f>SUM(F39:F42)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="84">
+      <c r="G38" s="83">
         <f>SUM(G39:G42)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="89"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="87"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="86"/>
       <c r="K38" s="73"/>
     </row>
     <row r="39" spans="1:12" s="66" customFormat="1">
-      <c r="A39" s="100"/>
-      <c r="B39" s="98" t="s">
+      <c r="A39" s="99"/>
+      <c r="B39" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="110">
+      <c r="C39" s="109">
         <f t="shared" ref="C39:C46" si="0">SUM(D39:G39)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="134"/>
-      <c r="I39" s="137"/>
-      <c r="J39" s="99"/>
+      <c r="D39" s="247"/>
+      <c r="E39" s="247"/>
+      <c r="F39" s="247"/>
+      <c r="G39" s="247"/>
+      <c r="H39" s="132"/>
+      <c r="I39" s="135"/>
+      <c r="J39" s="98"/>
       <c r="K39" s="69"/>
     </row>
     <row r="40" spans="1:12" s="66" customFormat="1">
-      <c r="A40" s="100"/>
-      <c r="B40" s="98" t="s">
+      <c r="A40" s="99"/>
+      <c r="B40" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="110">
+      <c r="C40" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="134"/>
-      <c r="I40" s="137"/>
-      <c r="J40" s="99"/>
+      <c r="D40" s="247"/>
+      <c r="E40" s="247"/>
+      <c r="F40" s="247"/>
+      <c r="G40" s="247"/>
+      <c r="H40" s="132"/>
+      <c r="I40" s="135"/>
+      <c r="J40" s="98"/>
       <c r="K40" s="69"/>
     </row>
     <row r="41" spans="1:12" s="66" customFormat="1">
-      <c r="A41" s="100"/>
-      <c r="B41" s="98" t="s">
+      <c r="A41" s="99"/>
+      <c r="B41" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="110">
+      <c r="C41" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="134"/>
-      <c r="I41" s="137"/>
-      <c r="J41" s="99"/>
+      <c r="D41" s="247"/>
+      <c r="E41" s="247"/>
+      <c r="F41" s="247"/>
+      <c r="G41" s="247"/>
+      <c r="H41" s="132"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="98"/>
       <c r="K41" s="69"/>
     </row>
     <row r="42" spans="1:12" s="66" customFormat="1">
-      <c r="A42" s="100"/>
-      <c r="B42" s="98" t="s">
+      <c r="A42" s="99"/>
+      <c r="B42" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="110">
+      <c r="C42" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="134"/>
-      <c r="I42" s="137"/>
-      <c r="J42" s="99"/>
+      <c r="D42" s="247"/>
+      <c r="E42" s="247"/>
+      <c r="F42" s="247"/>
+      <c r="G42" s="247"/>
+      <c r="H42" s="132"/>
+      <c r="I42" s="135"/>
+      <c r="J42" s="98"/>
       <c r="K42" s="69"/>
     </row>
     <row r="43" spans="1:12" s="72" customFormat="1">
-      <c r="A43" s="88">
+      <c r="A43" s="87">
         <f>+A38+1</f>
         <v>6</v>
       </c>
-      <c r="B43" s="146" t="s">
+      <c r="B43" s="144" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="84">
+      <c r="C43" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D43" s="84">
+      <c r="D43" s="83">
         <f>SUM(D44:D46)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="84">
+      <c r="E43" s="83">
         <f>SUM(E44:E46)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="84">
+      <c r="F43" s="83">
         <f>SUM(F44:F46)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="84">
+      <c r="G43" s="83">
         <f>SUM(G44:G46)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="89"/>
-      <c r="I43" s="90"/>
-      <c r="J43" s="87"/>
+      <c r="H43" s="88"/>
+      <c r="I43" s="89"/>
+      <c r="J43" s="86"/>
       <c r="K43" s="73"/>
     </row>
     <row r="44" spans="1:12" s="66" customFormat="1">
-      <c r="A44" s="100"/>
-      <c r="B44" s="98" t="s">
+      <c r="A44" s="99"/>
+      <c r="B44" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="110">
+      <c r="C44" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="134"/>
-      <c r="I44" s="137"/>
-      <c r="J44" s="99"/>
+      <c r="D44" s="247"/>
+      <c r="E44" s="247"/>
+      <c r="F44" s="247"/>
+      <c r="G44" s="247"/>
+      <c r="H44" s="132"/>
+      <c r="I44" s="135"/>
+      <c r="J44" s="98"/>
       <c r="K44" s="69"/>
     </row>
     <row r="45" spans="1:12" s="66" customFormat="1">
       <c r="A45" s="74"/>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="110">
+      <c r="C45" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="134"/>
-      <c r="I45" s="137"/>
-      <c r="J45" s="99"/>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="132"/>
+      <c r="I45" s="135"/>
+      <c r="J45" s="98"/>
       <c r="K45" s="69"/>
     </row>
     <row r="46" spans="1:12" s="66" customFormat="1">
-      <c r="A46" s="100"/>
-      <c r="B46" s="98" t="s">
+      <c r="A46" s="99"/>
+      <c r="B46" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="110">
+      <c r="C46" s="109">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="134"/>
-      <c r="I46" s="137"/>
-      <c r="J46" s="99"/>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="132"/>
+      <c r="I46" s="135"/>
+      <c r="J46" s="98"/>
       <c r="K46" s="69"/>
     </row>
     <row r="47" spans="1:12" s="77" customFormat="1">
-      <c r="A47" s="227" t="s">
+      <c r="A47" s="218" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="228"/>
-      <c r="C47" s="91">
+      <c r="B47" s="219"/>
+      <c r="C47" s="90">
         <f>+C43+C38+C36+C34+C32+C19+C15</f>
         <v>0</v>
       </c>
-      <c r="D47" s="91">
+      <c r="D47" s="90">
         <f>+D43+D38+D36+D34+D32+D19+D15</f>
         <v>0</v>
       </c>
-      <c r="E47" s="91">
+      <c r="E47" s="90">
         <f>+E43+E38+E36+E34+E32+E19+E15</f>
         <v>0</v>
       </c>
-      <c r="F47" s="91">
+      <c r="F47" s="90">
         <f>+F43+F38+F36+F34+F32+F19+F15</f>
         <v>0</v>
       </c>
-      <c r="G47" s="91">
+      <c r="G47" s="90">
         <f>+G43+G38+G36+G34+G32+G19+G15</f>
         <v>0</v>
       </c>
-      <c r="H47" s="92"/>
-      <c r="I47" s="93"/>
-      <c r="J47" s="93"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="92"/>
       <c r="K47" s="80"/>
-      <c r="L47" s="94"/>
+      <c r="L47" s="93"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="49"/>
@@ -4249,8 +4277,8 @@
     <row r="54" spans="1:12" s="44" customFormat="1">
       <c r="A54" s="56"/>
       <c r="B54" s="54"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="109"/>
+      <c r="C54" s="103"/>
+      <c r="D54" s="108"/>
       <c r="E54" s="53"/>
       <c r="F54" s="53"/>
       <c r="G54" s="53"/>
@@ -4263,8 +4291,8 @@
     <row r="55" spans="1:12">
       <c r="A55" s="50"/>
       <c r="B55" s="54"/>
-      <c r="C55" s="117"/>
-      <c r="D55" s="109"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="108"/>
       <c r="E55" s="52"/>
       <c r="F55" s="52"/>
       <c r="G55" s="52"/>
@@ -4277,8 +4305,8 @@
     <row r="56" spans="1:12">
       <c r="A56" s="50"/>
       <c r="B56" s="49"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="119"/>
+      <c r="C56" s="117"/>
+      <c r="D56" s="118"/>
       <c r="E56" s="52"/>
       <c r="F56" s="52"/>
       <c r="G56" s="52"/>
@@ -4290,22 +4318,16 @@
     </row>
     <row r="57" spans="1:12">
       <c r="B57" s="49"/>
-      <c r="C57" s="120"/>
-      <c r="D57" s="119"/>
+      <c r="C57" s="119"/>
+      <c r="D57" s="118"/>
     </row>
     <row r="59" spans="1:12">
-      <c r="B59" s="122"/>
-      <c r="C59" s="118"/>
-      <c r="D59" s="119"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="117"/>
+      <c r="D59" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="A15:A31"/>
-    <mergeCell ref="B20:I20"/>
     <mergeCell ref="A8:J8"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A9:J9"/>
@@ -4319,6 +4341,12 @@
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="G12:G14"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="A15:A31"/>
+    <mergeCell ref="B20:I20"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244093999" right="0.23622047244093999" top="0.59055118110236005" bottom="0.59055118110236005" header="0.31496062992126" footer="0.31496062992126"/>
@@ -4331,8 +4359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D44" sqref="D44:G46"/>
     </sheetView>
   </sheetViews>
@@ -4340,11 +4368,11 @@
   <cols>
     <col min="1" max="1" width="5.28515625" style="62" customWidth="1"/>
     <col min="2" max="2" width="48.42578125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="150" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="148" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="66" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="66" customWidth="1"/>
     <col min="6" max="7" width="16" style="66" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="165" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="163" customWidth="1"/>
     <col min="9" max="9" width="18" style="62" customWidth="1"/>
     <col min="10" max="10" width="28.140625" style="62" customWidth="1"/>
     <col min="11" max="11" width="15" style="62" customWidth="1"/>
@@ -4352,449 +4380,449 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:12">
-      <c r="A7" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="220"/>
-      <c r="C7" s="220"/>
-      <c r="D7" s="220"/>
-      <c r="E7" s="220"/>
-      <c r="F7" s="220"/>
-      <c r="G7" s="220"/>
-      <c r="H7" s="220"/>
-      <c r="I7" s="220"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="147"/>
+      <c r="A7" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="227"/>
+      <c r="C7" s="227"/>
+      <c r="D7" s="227"/>
+      <c r="E7" s="227"/>
+      <c r="F7" s="227"/>
+      <c r="G7" s="227"/>
+      <c r="H7" s="227"/>
+      <c r="I7" s="227"/>
+      <c r="J7" s="227"/>
+      <c r="K7" s="145"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="227" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="220"/>
-      <c r="C8" s="220"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="220"/>
-      <c r="F8" s="220"/>
-      <c r="G8" s="220"/>
-      <c r="H8" s="220"/>
-      <c r="I8" s="220"/>
-      <c r="J8" s="220"/>
-      <c r="K8" s="147"/>
+      <c r="B8" s="227"/>
+      <c r="C8" s="227"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="227"/>
+      <c r="G8" s="227"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="227"/>
+      <c r="K8" s="145"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="220" t="s">
+      <c r="A9" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="220"/>
-      <c r="C9" s="220"/>
-      <c r="D9" s="220"/>
-      <c r="E9" s="220"/>
-      <c r="F9" s="220"/>
-      <c r="G9" s="220"/>
-      <c r="H9" s="220"/>
-      <c r="I9" s="220"/>
-      <c r="J9" s="220"/>
-      <c r="K9" s="147"/>
+      <c r="B9" s="227"/>
+      <c r="C9" s="227"/>
+      <c r="D9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="227"/>
+      <c r="H9" s="227"/>
+      <c r="I9" s="227"/>
+      <c r="J9" s="227"/>
+      <c r="K9" s="145"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="220" t="s">
+      <c r="A10" s="227" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="220"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="220"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="220"/>
-      <c r="K10" s="147"/>
+      <c r="B10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="227"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="227"/>
+      <c r="K10" s="145"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A11" s="148"/>
-      <c r="B11" s="149" t="s">
+      <c r="A11" s="146"/>
+      <c r="B11" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="151"/>
-      <c r="F11" s="151"/>
-      <c r="G11" s="151"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="153" t="s">
+      <c r="E11" s="149"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="151" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="154"/>
-      <c r="K11" s="148"/>
-      <c r="L11" s="148"/>
+      <c r="J11" s="152"/>
+      <c r="K11" s="146"/>
+      <c r="L11" s="146"/>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1">
-      <c r="A12" s="246" t="s">
+      <c r="A12" s="230" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="234" t="s">
+      <c r="B12" s="233" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="234" t="s">
+      <c r="C12" s="233" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="234" t="s">
+      <c r="D12" s="233" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="234" t="s">
+      <c r="E12" s="233" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="237" t="s">
+      <c r="F12" s="238" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="237" t="s">
+      <c r="G12" s="238" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="237" t="s">
+      <c r="H12" s="238" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="234" t="s">
+      <c r="I12" s="233" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="240" t="s">
+      <c r="J12" s="241" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="221"/>
-      <c r="L12" s="221"/>
+      <c r="K12" s="223"/>
+      <c r="L12" s="223"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="247"/>
-      <c r="B13" s="235"/>
-      <c r="C13" s="235"/>
-      <c r="D13" s="235"/>
-      <c r="E13" s="235"/>
-      <c r="F13" s="238"/>
-      <c r="G13" s="238"/>
-      <c r="H13" s="238"/>
-      <c r="I13" s="235"/>
-      <c r="J13" s="241"/>
-      <c r="K13" s="221"/>
-      <c r="L13" s="221"/>
+      <c r="A13" s="231"/>
+      <c r="B13" s="234"/>
+      <c r="C13" s="234"/>
+      <c r="D13" s="234"/>
+      <c r="E13" s="234"/>
+      <c r="F13" s="239"/>
+      <c r="G13" s="239"/>
+      <c r="H13" s="239"/>
+      <c r="I13" s="234"/>
+      <c r="J13" s="242"/>
+      <c r="K13" s="223"/>
+      <c r="L13" s="223"/>
     </row>
     <row r="14" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A14" s="248"/>
-      <c r="B14" s="236"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
-      <c r="E14" s="236"/>
-      <c r="F14" s="239"/>
-      <c r="G14" s="239"/>
-      <c r="H14" s="239"/>
-      <c r="I14" s="236"/>
-      <c r="J14" s="242"/>
-      <c r="K14" s="221"/>
-      <c r="L14" s="221"/>
+      <c r="A14" s="232"/>
+      <c r="B14" s="235"/>
+      <c r="C14" s="235"/>
+      <c r="D14" s="235"/>
+      <c r="E14" s="235"/>
+      <c r="F14" s="240"/>
+      <c r="G14" s="240"/>
+      <c r="H14" s="240"/>
+      <c r="I14" s="235"/>
+      <c r="J14" s="243"/>
+      <c r="K14" s="223"/>
+      <c r="L14" s="223"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="243">
+      <c r="A15" s="244">
         <v>1</v>
       </c>
-      <c r="B15" s="166" t="s">
+      <c r="B15" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="167">
+      <c r="C15" s="165">
         <f>SUM(C16:C18)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="167">
+      <c r="D15" s="165">
         <f>SUM(D16:D18)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="167">
+      <c r="E15" s="165">
         <f>SUM(E16:E18)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="167">
+      <c r="F15" s="165">
         <f>SUM(F16:F18)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="167">
+      <c r="G15" s="165">
         <f>SUM(G16:G18)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="168"/>
-      <c r="I15" s="169"/>
-      <c r="J15" s="170"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="168"/>
       <c r="K15" s="61"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="244"/>
+      <c r="A16" s="245"/>
       <c r="B16" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="111">
+      <c r="C16" s="110">
         <f>SUM(D16:G16)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="155"/>
-      <c r="I16" s="156"/>
+      <c r="D16" s="247"/>
+      <c r="E16" s="247"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="247"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="154"/>
       <c r="J16" s="60"/>
       <c r="K16" s="61"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="244"/>
+      <c r="A17" s="245"/>
       <c r="B17" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="111">
+      <c r="C17" s="110">
         <f>SUM(D17:G17)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="155"/>
-      <c r="I17" s="156"/>
+      <c r="D17" s="247"/>
+      <c r="E17" s="247"/>
+      <c r="F17" s="247"/>
+      <c r="G17" s="247"/>
+      <c r="H17" s="153"/>
+      <c r="I17" s="154"/>
       <c r="J17" s="60"/>
       <c r="K17" s="61"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="244"/>
+      <c r="A18" s="245"/>
       <c r="B18" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="111">
+      <c r="C18" s="110">
         <f>SUM(D18:G18)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="155"/>
-      <c r="I18" s="156"/>
+      <c r="D18" s="247"/>
+      <c r="E18" s="247"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="247"/>
+      <c r="H18" s="153"/>
+      <c r="I18" s="154"/>
       <c r="J18" s="60"/>
       <c r="K18" s="61"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="244"/>
-      <c r="B19" s="171" t="s">
+      <c r="A19" s="245"/>
+      <c r="B19" s="169" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="172">
+      <c r="C19" s="170">
         <f>+C21+C23+C24+C26+C27+C29+C31</f>
         <v>0</v>
       </c>
-      <c r="D19" s="172">
+      <c r="D19" s="170">
         <f>+D21+D23+D24+D26+D27+D29+D31</f>
         <v>0</v>
       </c>
-      <c r="E19" s="172">
+      <c r="E19" s="170">
         <f>SUM(E20:E31)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="172">
+      <c r="F19" s="170">
         <f>SUM(F20:F31)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="172">
+      <c r="G19" s="170">
         <f>SUM(G20:G31)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="173"/>
-      <c r="I19" s="174"/>
-      <c r="J19" s="175"/>
+      <c r="H19" s="171"/>
+      <c r="I19" s="172"/>
+      <c r="J19" s="173"/>
       <c r="K19" s="61"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="244"/>
-      <c r="B20" s="158" t="s">
+      <c r="A20" s="245"/>
+      <c r="B20" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="159"/>
-      <c r="D20" s="160"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="160"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="158"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
+      <c r="H20" s="159"/>
+      <c r="I20" s="155"/>
       <c r="J20" s="75"/>
       <c r="K20" s="61"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="244"/>
+      <c r="A21" s="245"/>
       <c r="B21" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="111">
+      <c r="C21" s="110">
         <f>SUM(D21:G21)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="137"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="247"/>
+      <c r="F21" s="247"/>
+      <c r="G21" s="247"/>
+      <c r="H21" s="132"/>
+      <c r="I21" s="135"/>
       <c r="J21" s="60"/>
       <c r="K21" s="61"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="244"/>
-      <c r="B22" s="95" t="s">
+      <c r="A22" s="245"/>
+      <c r="B22" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="106"/>
+      <c r="C22" s="105"/>
       <c r="D22" s="69"/>
       <c r="E22" s="69"/>
       <c r="F22" s="69"/>
       <c r="G22" s="69"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="96"/>
+      <c r="H22" s="133"/>
+      <c r="I22" s="95"/>
       <c r="J22" s="75"/>
       <c r="K22" s="61"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="244"/>
+      <c r="A23" s="245"/>
       <c r="B23" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="111">
+      <c r="C23" s="110">
         <f>SUM(D23:G23)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="137"/>
+      <c r="D23" s="247"/>
+      <c r="E23" s="247"/>
+      <c r="F23" s="247"/>
+      <c r="G23" s="247"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="135"/>
       <c r="J23" s="60"/>
       <c r="K23" s="61"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="244"/>
+      <c r="A24" s="245"/>
       <c r="B24" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="111">
+      <c r="C24" s="110">
         <f>SUM(D24:G24)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="134"/>
-      <c r="I24" s="137"/>
+      <c r="D24" s="247"/>
+      <c r="E24" s="247"/>
+      <c r="F24" s="247"/>
+      <c r="G24" s="247"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="135"/>
       <c r="J24" s="60"/>
       <c r="K24" s="61"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="244"/>
-      <c r="B25" s="95" t="s">
+      <c r="A25" s="245"/>
+      <c r="B25" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="106"/>
+      <c r="C25" s="105"/>
       <c r="D25" s="69"/>
       <c r="E25" s="69"/>
       <c r="F25" s="69"/>
       <c r="G25" s="69"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="96"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="95"/>
       <c r="J25" s="75"/>
       <c r="K25" s="61"/>
     </row>
     <row r="26" spans="1:16" s="66" customFormat="1">
-      <c r="A26" s="244"/>
+      <c r="A26" s="245"/>
       <c r="B26" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="111">
+      <c r="C26" s="110">
         <f>SUM(D26:G26)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="134"/>
-      <c r="I26" s="137"/>
+      <c r="D26" s="247"/>
+      <c r="E26" s="247"/>
+      <c r="F26" s="247"/>
+      <c r="G26" s="247"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="135"/>
       <c r="J26" s="64"/>
       <c r="K26" s="61"/>
       <c r="L26" s="62"/>
     </row>
     <row r="27" spans="1:16" s="66" customFormat="1">
-      <c r="A27" s="244"/>
+      <c r="A27" s="245"/>
       <c r="B27" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="111">
+      <c r="C27" s="110">
         <f>SUM(D27:G27)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="134"/>
-      <c r="I27" s="137"/>
+      <c r="D27" s="247"/>
+      <c r="E27" s="247"/>
+      <c r="F27" s="247"/>
+      <c r="G27" s="247"/>
+      <c r="H27" s="132"/>
+      <c r="I27" s="135"/>
       <c r="J27" s="64"/>
       <c r="K27" s="69"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="244"/>
-      <c r="B28" s="95" t="s">
+      <c r="A28" s="245"/>
+      <c r="B28" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="106"/>
+      <c r="C28" s="105"/>
       <c r="D28" s="69"/>
       <c r="E28" s="69"/>
       <c r="F28" s="69"/>
       <c r="G28" s="69"/>
-      <c r="H28" s="135"/>
-      <c r="I28" s="96"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="95"/>
       <c r="J28" s="75"/>
       <c r="K28" s="61"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="244"/>
+      <c r="A29" s="245"/>
       <c r="B29" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="100">
+      <c r="C29" s="99">
         <f>SUM(D29:G29)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="134"/>
-      <c r="I29" s="137"/>
-      <c r="J29" s="112"/>
+      <c r="D29" s="247"/>
+      <c r="E29" s="247"/>
+      <c r="F29" s="247"/>
+      <c r="G29" s="247"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="135"/>
+      <c r="J29" s="111"/>
       <c r="K29" s="61"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="244"/>
-      <c r="B30" s="95" t="s">
+      <c r="A30" s="245"/>
+      <c r="B30" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="106"/>
+      <c r="C30" s="105"/>
       <c r="D30" s="69"/>
       <c r="E30" s="69"/>
       <c r="F30" s="69"/>
       <c r="G30" s="69"/>
-      <c r="H30" s="135"/>
-      <c r="I30" s="96"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="95"/>
       <c r="J30" s="75"/>
       <c r="K30" s="61"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="245"/>
-      <c r="B31" s="162" t="s">
+      <c r="A31" s="246"/>
+      <c r="B31" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="111">
+      <c r="C31" s="110">
         <f>SUM(D31:G31)</f>
         <v>0</v>
       </c>
@@ -4802,214 +4830,214 @@
       <c r="E31" s="65"/>
       <c r="F31" s="65"/>
       <c r="G31" s="65"/>
-      <c r="H31" s="134"/>
-      <c r="I31" s="137"/>
-      <c r="J31" s="124"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="135"/>
+      <c r="J31" s="123"/>
       <c r="K31" s="61"/>
-      <c r="O31" s="135"/>
+      <c r="O31" s="133"/>
       <c r="P31" s="61"/>
     </row>
-    <row r="32" spans="1:16" s="183" customFormat="1">
-      <c r="A32" s="176">
+    <row r="32" spans="1:16" s="181" customFormat="1">
+      <c r="A32" s="174">
         <f>+A15+1</f>
         <v>2</v>
       </c>
-      <c r="B32" s="177" t="s">
+      <c r="B32" s="175" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="178">
+      <c r="C32" s="176">
         <f>+C33</f>
         <v>0</v>
       </c>
-      <c r="D32" s="178">
+      <c r="D32" s="176">
         <f>+D33</f>
         <v>0</v>
       </c>
-      <c r="E32" s="178">
+      <c r="E32" s="176">
         <f>+E33</f>
         <v>0</v>
       </c>
-      <c r="F32" s="178">
+      <c r="F32" s="176">
         <f>+F33</f>
         <v>0</v>
       </c>
-      <c r="G32" s="178">
+      <c r="G32" s="176">
         <f>+G33</f>
         <v>0</v>
       </c>
-      <c r="H32" s="179"/>
-      <c r="I32" s="180"/>
-      <c r="J32" s="181"/>
-      <c r="K32" s="182"/>
+      <c r="H32" s="177"/>
+      <c r="I32" s="178"/>
+      <c r="J32" s="179"/>
+      <c r="K32" s="180"/>
     </row>
     <row r="33" spans="1:12" s="66" customFormat="1" ht="30" customHeight="1">
-      <c r="A33" s="113"/>
-      <c r="B33" s="114" t="s">
+      <c r="A33" s="112"/>
+      <c r="B33" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="111">
+      <c r="C33" s="110">
         <f>SUM(D33:G33)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="134"/>
-      <c r="I33" s="137"/>
+      <c r="D33" s="247"/>
+      <c r="E33" s="247"/>
+      <c r="F33" s="247"/>
+      <c r="G33" s="247"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="135"/>
       <c r="J33" s="67"/>
       <c r="K33" s="68"/>
     </row>
-    <row r="34" spans="1:12" s="183" customFormat="1">
-      <c r="A34" s="184">
+    <row r="34" spans="1:12" s="181" customFormat="1">
+      <c r="A34" s="182">
         <f>+A32+1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="185" t="s">
+      <c r="B34" s="183" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="167">
+      <c r="C34" s="165">
         <f>+C35</f>
         <v>0</v>
       </c>
-      <c r="D34" s="167">
+      <c r="D34" s="165">
         <f>+D35</f>
         <v>0</v>
       </c>
-      <c r="E34" s="167">
+      <c r="E34" s="165">
         <f>SUM(E35)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="167">
+      <c r="F34" s="165">
         <f>+F35</f>
         <v>0</v>
       </c>
-      <c r="G34" s="167">
+      <c r="G34" s="165">
         <f>+G35</f>
         <v>0</v>
       </c>
-      <c r="H34" s="186"/>
-      <c r="I34" s="187"/>
-      <c r="J34" s="170"/>
-      <c r="K34" s="182"/>
+      <c r="H34" s="184"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="168"/>
+      <c r="K34" s="180"/>
     </row>
     <row r="35" spans="1:12" s="66" customFormat="1">
-      <c r="A35" s="111"/>
+      <c r="A35" s="110"/>
       <c r="B35" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="111">
+      <c r="C35" s="110">
         <f>SUM(D35:G35)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="134"/>
-      <c r="I35" s="137"/>
+      <c r="D35" s="247"/>
+      <c r="E35" s="247"/>
+      <c r="F35" s="247"/>
+      <c r="G35" s="247"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="135"/>
       <c r="J35" s="64"/>
       <c r="K35" s="69"/>
     </row>
-    <row r="36" spans="1:12" s="183" customFormat="1">
-      <c r="A36" s="188">
+    <row r="36" spans="1:12" s="181" customFormat="1">
+      <c r="A36" s="186">
         <f>+A34+1</f>
         <v>4</v>
       </c>
-      <c r="B36" s="189" t="s">
+      <c r="B36" s="187" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="172">
+      <c r="C36" s="170">
         <f>+C37</f>
         <v>0</v>
       </c>
-      <c r="D36" s="172">
+      <c r="D36" s="170">
         <f>+D37</f>
         <v>0</v>
       </c>
-      <c r="E36" s="172">
+      <c r="E36" s="170">
         <f>+E37</f>
         <v>0</v>
       </c>
-      <c r="F36" s="172">
+      <c r="F36" s="170">
         <f>+F37</f>
         <v>0</v>
       </c>
-      <c r="G36" s="172">
+      <c r="G36" s="170">
         <f>+G37</f>
         <v>0</v>
       </c>
-      <c r="H36" s="190"/>
-      <c r="I36" s="191"/>
-      <c r="J36" s="181"/>
-      <c r="K36" s="182"/>
+      <c r="H36" s="188"/>
+      <c r="I36" s="189"/>
+      <c r="J36" s="179"/>
+      <c r="K36" s="180"/>
     </row>
     <row r="37" spans="1:12" s="66" customFormat="1">
-      <c r="A37" s="111"/>
+      <c r="A37" s="110"/>
       <c r="B37" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="111">
+      <c r="C37" s="110">
         <f>SUM(D37:G37)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="134"/>
-      <c r="I37" s="137"/>
+      <c r="D37" s="247"/>
+      <c r="E37" s="247"/>
+      <c r="F37" s="247"/>
+      <c r="G37" s="247"/>
+      <c r="H37" s="132"/>
+      <c r="I37" s="135"/>
       <c r="J37" s="64"/>
       <c r="K37" s="69"/>
     </row>
-    <row r="38" spans="1:12" s="183" customFormat="1">
-      <c r="A38" s="188">
+    <row r="38" spans="1:12" s="181" customFormat="1">
+      <c r="A38" s="186">
         <f>+A36+1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="189" t="s">
+      <c r="B38" s="187" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="178">
+      <c r="C38" s="176">
         <f>SUM(C39:C42)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="178">
+      <c r="D38" s="176">
         <f>SUM(D39:D42)</f>
         <v>0</v>
       </c>
-      <c r="E38" s="178">
+      <c r="E38" s="176">
         <f>SUM(E39:E42)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="178">
+      <c r="F38" s="176">
         <f>SUM(F39:F42)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="178">
+      <c r="G38" s="176">
         <f>SUM(G39:G42)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="190"/>
-      <c r="I38" s="191"/>
-      <c r="J38" s="181"/>
-      <c r="K38" s="182"/>
+      <c r="H38" s="188"/>
+      <c r="I38" s="189"/>
+      <c r="J38" s="179"/>
+      <c r="K38" s="180"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="63"/>
       <c r="B39" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="111">
+      <c r="C39" s="110">
         <f>SUM(D39:G39)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="134"/>
-      <c r="I39" s="137"/>
+      <c r="D39" s="247"/>
+      <c r="E39" s="247"/>
+      <c r="F39" s="247"/>
+      <c r="G39" s="247"/>
+      <c r="H39" s="132"/>
+      <c r="I39" s="135"/>
       <c r="J39" s="60"/>
       <c r="K39" s="61"/>
     </row>
@@ -5018,16 +5046,16 @@
       <c r="B40" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="111">
+      <c r="C40" s="110">
         <f>SUM(D40:G40)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="134"/>
-      <c r="I40" s="137"/>
+      <c r="D40" s="247"/>
+      <c r="E40" s="247"/>
+      <c r="F40" s="247"/>
+      <c r="G40" s="247"/>
+      <c r="H40" s="132"/>
+      <c r="I40" s="135"/>
       <c r="J40" s="60"/>
       <c r="K40" s="61"/>
     </row>
@@ -5036,16 +5064,16 @@
       <c r="B41" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="111">
+      <c r="C41" s="110">
         <f>SUM(D41:G41)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="134"/>
-      <c r="I41" s="137"/>
+      <c r="D41" s="247"/>
+      <c r="E41" s="247"/>
+      <c r="F41" s="247"/>
+      <c r="G41" s="247"/>
+      <c r="H41" s="132"/>
+      <c r="I41" s="135"/>
       <c r="J41" s="60"/>
       <c r="K41" s="61"/>
     </row>
@@ -5054,268 +5082,260 @@
       <c r="B42" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="111">
+      <c r="C42" s="110">
         <f>SUM(D42:G42)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="134"/>
-      <c r="I42" s="137"/>
+      <c r="D42" s="247"/>
+      <c r="E42" s="247"/>
+      <c r="F42" s="247"/>
+      <c r="G42" s="247"/>
+      <c r="H42" s="132"/>
+      <c r="I42" s="135"/>
       <c r="J42" s="60"/>
       <c r="K42" s="61"/>
     </row>
-    <row r="43" spans="1:12" s="183" customFormat="1">
-      <c r="A43" s="188">
+    <row r="43" spans="1:12" s="181" customFormat="1">
+      <c r="A43" s="186">
         <f>+A38+1</f>
         <v>6</v>
       </c>
-      <c r="B43" s="189" t="s">
+      <c r="B43" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="178">
+      <c r="C43" s="176">
         <f>SUM(C44:C46)</f>
         <v>0</v>
       </c>
-      <c r="D43" s="178">
+      <c r="D43" s="176">
         <f>SUM(D44:D46)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="178">
+      <c r="E43" s="176">
         <f>SUM(E44:E46)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="178">
+      <c r="F43" s="176">
         <f>SUM(F44:F46)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="178">
+      <c r="G43" s="176">
         <f>SUM(G44:G46)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="190"/>
-      <c r="I43" s="191"/>
-      <c r="J43" s="181"/>
-      <c r="K43" s="182"/>
+      <c r="H43" s="188"/>
+      <c r="I43" s="189"/>
+      <c r="J43" s="179"/>
+      <c r="K43" s="180"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="115"/>
+      <c r="A44" s="114"/>
       <c r="B44" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="111">
+      <c r="C44" s="110">
         <f>SUM(D44:G44)</f>
         <v>0</v>
       </c>
-      <c r="D44" s="64"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="134"/>
-      <c r="I44" s="137"/>
+      <c r="D44" s="247"/>
+      <c r="E44" s="247"/>
+      <c r="F44" s="247"/>
+      <c r="G44" s="247"/>
+      <c r="H44" s="132"/>
+      <c r="I44" s="135"/>
       <c r="J44" s="64"/>
       <c r="K44" s="61"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="116"/>
+      <c r="A45" s="115"/>
       <c r="B45" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="111">
+      <c r="C45" s="110">
         <f>SUM(D45:G45)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="134"/>
-      <c r="I45" s="137"/>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="132"/>
+      <c r="I45" s="135"/>
       <c r="J45" s="60"/>
       <c r="K45" s="61"/>
     </row>
     <row r="46" spans="1:12" s="66" customFormat="1">
-      <c r="A46" s="100"/>
+      <c r="A46" s="99"/>
       <c r="B46" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="111">
+      <c r="C46" s="110">
         <f>SUM(D46:G46)</f>
         <v>0</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="134"/>
-      <c r="I46" s="137"/>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="132"/>
+      <c r="I46" s="135"/>
       <c r="J46" s="64"/>
       <c r="K46" s="69"/>
     </row>
-    <row r="47" spans="1:12" s="197" customFormat="1">
-      <c r="A47" s="232" t="s">
+    <row r="47" spans="1:12" s="195" customFormat="1">
+      <c r="A47" s="236" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="233"/>
-      <c r="C47" s="192">
+      <c r="B47" s="237"/>
+      <c r="C47" s="190">
         <f>+C43+C38+C36+C34+C32+C19+C15</f>
         <v>0</v>
       </c>
-      <c r="D47" s="192">
+      <c r="D47" s="190">
         <f>+D43+D38+D36+D34+D32+D19+D15</f>
         <v>0</v>
       </c>
-      <c r="E47" s="192">
+      <c r="E47" s="190">
         <f>+E43+E38+E36+E34+E32+E19+E15</f>
         <v>0</v>
       </c>
-      <c r="F47" s="192">
+      <c r="F47" s="190">
         <f>+F43+F38+F36+F34+F32+F19+F15</f>
         <v>0</v>
       </c>
-      <c r="G47" s="192">
+      <c r="G47" s="190">
         <f>+G43+G38+G36+G34+G32+G19+G15</f>
         <v>0</v>
       </c>
-      <c r="H47" s="193"/>
-      <c r="I47" s="194"/>
-      <c r="J47" s="194"/>
-      <c r="K47" s="195"/>
-      <c r="L47" s="196"/>
+      <c r="H47" s="191"/>
+      <c r="I47" s="192"/>
+      <c r="J47" s="192"/>
+      <c r="K47" s="193"/>
+      <c r="L47" s="194"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="163"/>
-      <c r="B48" s="163"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="108"/>
-      <c r="E48" s="108"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="108"/>
-      <c r="H48" s="136"/>
+      <c r="A48" s="161"/>
+      <c r="B48" s="161"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="134"/>
       <c r="I48" s="52"/>
       <c r="J48" s="52"/>
-      <c r="K48" s="163"/>
-      <c r="L48" s="164"/>
+      <c r="K48" s="161"/>
+      <c r="L48" s="162"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="163"/>
-      <c r="B49" s="163"/>
-      <c r="C49" s="103" t="s">
+      <c r="A49" s="161"/>
+      <c r="B49" s="161"/>
+      <c r="C49" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="108"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="136"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="107"/>
+      <c r="F49" s="107"/>
+      <c r="G49" s="107"/>
+      <c r="H49" s="134"/>
       <c r="I49" s="52"/>
       <c r="J49" s="52"/>
-      <c r="K49" s="163"/>
-      <c r="L49" s="164"/>
+      <c r="K49" s="161"/>
+      <c r="L49" s="162"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="163"/>
-      <c r="B50" s="163"/>
-      <c r="C50" s="103"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="108"/>
-      <c r="F50" s="108"/>
-      <c r="G50" s="108"/>
-      <c r="H50" s="136"/>
+      <c r="A50" s="161"/>
+      <c r="B50" s="161"/>
+      <c r="C50" s="102"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="107"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="134"/>
       <c r="I50" s="52"/>
       <c r="J50" s="52"/>
-      <c r="K50" s="163"/>
-      <c r="L50" s="164"/>
+      <c r="K50" s="161"/>
+      <c r="L50" s="162"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="164"/>
-      <c r="B51" s="163"/>
-      <c r="C51" s="103"/>
-      <c r="D51" s="108"/>
-      <c r="E51" s="108"/>
-      <c r="F51" s="108"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="136"/>
+      <c r="A51" s="162"/>
+      <c r="B51" s="161"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="107"/>
+      <c r="H51" s="134"/>
       <c r="I51" s="52"/>
       <c r="J51" s="52"/>
-      <c r="K51" s="164"/>
-      <c r="L51" s="164"/>
+      <c r="K51" s="162"/>
+      <c r="L51" s="162"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="164"/>
-      <c r="B52" s="163"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="108"/>
-      <c r="E52" s="108"/>
-      <c r="F52" s="108"/>
-      <c r="G52" s="108"/>
-      <c r="H52" s="136"/>
+      <c r="A52" s="162"/>
+      <c r="B52" s="161"/>
+      <c r="C52" s="102"/>
+      <c r="D52" s="107"/>
+      <c r="E52" s="107"/>
+      <c r="F52" s="107"/>
+      <c r="G52" s="107"/>
+      <c r="H52" s="134"/>
       <c r="I52" s="52"/>
       <c r="J52" s="52"/>
-      <c r="K52" s="164"/>
-      <c r="L52" s="164"/>
+      <c r="K52" s="162"/>
+      <c r="L52" s="162"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="164"/>
+      <c r="A53" s="162"/>
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
-      <c r="E53" s="108"/>
-      <c r="F53" s="108"/>
-      <c r="G53" s="108"/>
-      <c r="H53" s="136"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="107"/>
+      <c r="G53" s="107"/>
+      <c r="H53" s="134"/>
       <c r="I53" s="52"/>
       <c r="J53" s="52"/>
-      <c r="K53" s="164"/>
-      <c r="L53" s="164"/>
+      <c r="K53" s="162"/>
+      <c r="L53" s="162"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="164"/>
+      <c r="A54" s="162"/>
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
-      <c r="E54" s="108"/>
-      <c r="F54" s="108"/>
-      <c r="G54" s="108"/>
-      <c r="H54" s="136"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="107"/>
+      <c r="G54" s="107"/>
+      <c r="H54" s="134"/>
       <c r="I54" s="52"/>
       <c r="J54" s="52"/>
-      <c r="K54" s="164"/>
-      <c r="L54" s="164"/>
+      <c r="K54" s="162"/>
+      <c r="L54" s="162"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="164"/>
-      <c r="E55" s="108"/>
-      <c r="F55" s="108"/>
-      <c r="G55" s="108"/>
-      <c r="H55" s="136"/>
+      <c r="A55" s="162"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="107"/>
+      <c r="G55" s="107"/>
+      <c r="H55" s="134"/>
       <c r="I55" s="52"/>
       <c r="J55" s="52"/>
-      <c r="K55" s="164"/>
-      <c r="L55" s="164"/>
+      <c r="K55" s="162"/>
+      <c r="L55" s="162"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="164"/>
-      <c r="E56" s="108"/>
-      <c r="F56" s="108"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="136"/>
+      <c r="A56" s="162"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="107"/>
+      <c r="H56" s="134"/>
       <c r="I56" s="52"/>
       <c r="J56" s="52"/>
-      <c r="K56" s="164"/>
-      <c r="L56" s="164"/>
+      <c r="K56" s="162"/>
+      <c r="L56" s="162"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:J10"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
@@ -5326,6 +5346,14 @@
     <mergeCell ref="A15:A31"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="G12:G14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:J10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244093999" right="0.23622047244093999" top="0.19685039370078999" bottom="0.19685039370078999" header="0.39370078740157" footer="0.39370078740157"/>

</xml_diff>